<commit_message>
Rename products/industries in model aggregation
</commit_message>
<xml_diff>
--- a/project_example/00-principal/data/Eldata.xlsx
+++ b/project_example/00-principal/data/Eldata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="elasFU" sheetId="5" r:id="rId1"/>
@@ -19,216 +19,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
-    <t>i001</t>
-  </si>
-  <si>
-    <t>i002</t>
-  </si>
-  <si>
-    <t>i003</t>
-  </si>
-  <si>
-    <t>i004</t>
-  </si>
-  <si>
-    <t>i005</t>
-  </si>
-  <si>
-    <t>i006</t>
-  </si>
-  <si>
-    <t>i007</t>
-  </si>
-  <si>
-    <t>i008</t>
-  </si>
-  <si>
-    <t>i009</t>
-  </si>
-  <si>
-    <t>i010</t>
-  </si>
-  <si>
-    <t>i011</t>
-  </si>
-  <si>
-    <t>i012</t>
-  </si>
-  <si>
-    <t>i016</t>
-  </si>
-  <si>
-    <t>i020</t>
-  </si>
-  <si>
-    <t>i021</t>
-  </si>
-  <si>
-    <t>i022</t>
-  </si>
-  <si>
-    <t>i023</t>
-  </si>
-  <si>
-    <t>i024</t>
-  </si>
-  <si>
-    <t>i025</t>
-  </si>
-  <si>
-    <t>i026</t>
-  </si>
-  <si>
-    <t>i027</t>
-  </si>
-  <si>
-    <t>i028</t>
-  </si>
-  <si>
-    <t>i029</t>
-  </si>
-  <si>
-    <t>i030</t>
-  </si>
-  <si>
-    <t>i034</t>
-  </si>
-  <si>
-    <t>i042</t>
-  </si>
-  <si>
-    <t>i045</t>
-  </si>
-  <si>
-    <t>i046</t>
-  </si>
-  <si>
-    <t>i047</t>
-  </si>
-  <si>
-    <t>i048</t>
-  </si>
-  <si>
-    <t>i049</t>
-  </si>
-  <si>
-    <t>i050</t>
-  </si>
-  <si>
-    <t>i056</t>
-  </si>
-  <si>
-    <t>i057</t>
-  </si>
-  <si>
-    <t>i058</t>
-  </si>
-  <si>
-    <t>p001</t>
-  </si>
-  <si>
-    <t>p002</t>
-  </si>
-  <si>
-    <t>p003</t>
-  </si>
-  <si>
-    <t>p004</t>
-  </si>
-  <si>
-    <t>p005</t>
-  </si>
-  <si>
-    <t>p006</t>
-  </si>
-  <si>
-    <t>p007</t>
-  </si>
-  <si>
-    <t>p008</t>
-  </si>
-  <si>
-    <t>p009</t>
-  </si>
-  <si>
-    <t>p010</t>
-  </si>
-  <si>
-    <t>p011</t>
-  </si>
-  <si>
-    <t>p012</t>
-  </si>
-  <si>
-    <t>p016</t>
-  </si>
-  <si>
-    <t>p020</t>
-  </si>
-  <si>
-    <t>p021</t>
-  </si>
-  <si>
-    <t>p022</t>
-  </si>
-  <si>
-    <t>p023</t>
-  </si>
-  <si>
-    <t>p024</t>
-  </si>
-  <si>
-    <t>p025</t>
-  </si>
-  <si>
-    <t>p026</t>
-  </si>
-  <si>
-    <t>p027</t>
-  </si>
-  <si>
-    <t>p028</t>
-  </si>
-  <si>
-    <t>p029</t>
-  </si>
-  <si>
-    <t>p030</t>
-  </si>
-  <si>
-    <t>p034</t>
-  </si>
-  <si>
-    <t>p042</t>
-  </si>
-  <si>
-    <t>p045</t>
-  </si>
-  <si>
-    <t>p046</t>
-  </si>
-  <si>
-    <t>p047</t>
-  </si>
-  <si>
-    <t>p048</t>
-  </si>
-  <si>
-    <t>p049</t>
-  </si>
-  <si>
-    <t>p050</t>
-  </si>
-  <si>
-    <t>p056</t>
-  </si>
-  <si>
-    <t>p057</t>
-  </si>
-  <si>
-    <t>p058</t>
-  </si>
-  <si>
     <t>elasIU_DM</t>
   </si>
   <si>
@@ -263,6 +53,216 @@
   </si>
   <si>
     <t>GOS</t>
+  </si>
+  <si>
+    <t>pPARI</t>
+  </si>
+  <si>
+    <t>pWHEA</t>
+  </si>
+  <si>
+    <t>pOCER</t>
+  </si>
+  <si>
+    <t>pFVEG</t>
+  </si>
+  <si>
+    <t>pOILS</t>
+  </si>
+  <si>
+    <t>pSUGB</t>
+  </si>
+  <si>
+    <t>pFIBR</t>
+  </si>
+  <si>
+    <t>pOTHC</t>
+  </si>
+  <si>
+    <t>pANIM</t>
+  </si>
+  <si>
+    <t>pFORE</t>
+  </si>
+  <si>
+    <t>pFISH</t>
+  </si>
+  <si>
+    <t>pFOSM</t>
+  </si>
+  <si>
+    <t>pOTHM</t>
+  </si>
+  <si>
+    <t>pFBTO</t>
+  </si>
+  <si>
+    <t>pTXWO</t>
+  </si>
+  <si>
+    <t>pCOKE</t>
+  </si>
+  <si>
+    <t>pREFN</t>
+  </si>
+  <si>
+    <t>pCHEM</t>
+  </si>
+  <si>
+    <t>pRUBP</t>
+  </si>
+  <si>
+    <t>pNMMP</t>
+  </si>
+  <si>
+    <t>pMETP</t>
+  </si>
+  <si>
+    <t>pELEC</t>
+  </si>
+  <si>
+    <t>pMACH</t>
+  </si>
+  <si>
+    <t>pELCF</t>
+  </si>
+  <si>
+    <t>pELCG</t>
+  </si>
+  <si>
+    <t>pTRDI</t>
+  </si>
+  <si>
+    <t>pHWAT</t>
+  </si>
+  <si>
+    <t>pWATR</t>
+  </si>
+  <si>
+    <t>pCONS</t>
+  </si>
+  <si>
+    <t>pTRAD</t>
+  </si>
+  <si>
+    <t>pHORE</t>
+  </si>
+  <si>
+    <t>pTRAN</t>
+  </si>
+  <si>
+    <t>pREBA</t>
+  </si>
+  <si>
+    <t>pPUBO</t>
+  </si>
+  <si>
+    <t>pWAST</t>
+  </si>
+  <si>
+    <t>iPARI</t>
+  </si>
+  <si>
+    <t>iWHEA</t>
+  </si>
+  <si>
+    <t>iOCER</t>
+  </si>
+  <si>
+    <t>iFVEG</t>
+  </si>
+  <si>
+    <t>iOILS</t>
+  </si>
+  <si>
+    <t>iSUGB</t>
+  </si>
+  <si>
+    <t>iFIBR</t>
+  </si>
+  <si>
+    <t>iOTHC</t>
+  </si>
+  <si>
+    <t>iANIM</t>
+  </si>
+  <si>
+    <t>iFORE</t>
+  </si>
+  <si>
+    <t>iFISH</t>
+  </si>
+  <si>
+    <t>iFOSM</t>
+  </si>
+  <si>
+    <t>iOTHM</t>
+  </si>
+  <si>
+    <t>iFBTO</t>
+  </si>
+  <si>
+    <t>iTXWO</t>
+  </si>
+  <si>
+    <t>iCOKE</t>
+  </si>
+  <si>
+    <t>iREFN</t>
+  </si>
+  <si>
+    <t>iCHEM</t>
+  </si>
+  <si>
+    <t>iRUBP</t>
+  </si>
+  <si>
+    <t>iNMMP</t>
+  </si>
+  <si>
+    <t>iMETP</t>
+  </si>
+  <si>
+    <t>iELEC</t>
+  </si>
+  <si>
+    <t>iMACH</t>
+  </si>
+  <si>
+    <t>iELCF</t>
+  </si>
+  <si>
+    <t>iELCG</t>
+  </si>
+  <si>
+    <t>iTRDI</t>
+  </si>
+  <si>
+    <t>iHWAT</t>
+  </si>
+  <si>
+    <t>iWATR</t>
+  </si>
+  <si>
+    <t>iCONS</t>
+  </si>
+  <si>
+    <t>iTRAD</t>
+  </si>
+  <si>
+    <t>iHORE</t>
+  </si>
+  <si>
+    <t>iTRAN</t>
+  </si>
+  <si>
+    <t>iREBA</t>
+  </si>
+  <si>
+    <t>iPUBO</t>
+  </si>
+  <si>
+    <t>iWAST</t>
   </si>
 </sst>
 </file>
@@ -604,21 +604,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -626,7 +624,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -634,7 +632,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -642,7 +640,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -657,29 +655,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -696,7 +692,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -713,7 +709,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -730,7 +726,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -747,7 +743,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -764,7 +760,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -781,7 +777,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -798,7 +794,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -815,7 +811,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -832,7 +828,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -849,7 +845,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -866,7 +862,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -883,7 +879,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -900,7 +896,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -917,7 +913,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -934,7 +930,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -951,7 +947,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -968,7 +964,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>5</v>
@@ -985,7 +981,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>5</v>
@@ -1002,7 +998,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -1019,7 +1015,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>5</v>
@@ -1036,7 +1032,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>5</v>
@@ -1053,7 +1049,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>5</v>
@@ -1070,7 +1066,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>5</v>
@@ -1087,7 +1083,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -1104,7 +1100,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -1121,7 +1117,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -1138,7 +1134,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B29">
         <v>5</v>
@@ -1155,7 +1151,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>5</v>
@@ -1172,7 +1168,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="B31">
         <v>5</v>
@@ -1189,7 +1185,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="B32">
         <v>5</v>
@@ -1206,7 +1202,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B33">
         <v>5</v>
@@ -1223,7 +1219,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="B34">
         <v>5</v>
@@ -1240,7 +1236,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -1257,7 +1253,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="B36">
         <v>5</v>
@@ -1282,20 +1278,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>72</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>0.95</v>
@@ -1303,7 +1297,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>0.95</v>
@@ -1311,7 +1305,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>0.95</v>
@@ -1319,7 +1313,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>0.95</v>
@@ -1327,7 +1321,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <v>0.95</v>
@@ -1335,7 +1329,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>0.95</v>
@@ -1343,7 +1337,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>0.95</v>
@@ -1351,7 +1345,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>0.95</v>
@@ -1359,7 +1353,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="B10">
         <v>0.95</v>
@@ -1367,7 +1361,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B11">
         <v>0.95</v>
@@ -1375,7 +1369,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B12">
         <v>0.95</v>
@@ -1383,7 +1377,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>0.95</v>
@@ -1391,7 +1385,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="B14">
         <v>0.95</v>
@@ -1399,7 +1393,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B15">
         <v>0.95</v>
@@ -1407,7 +1401,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B16">
         <v>0.95</v>
@@ -1415,7 +1409,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B17">
         <v>0.95</v>
@@ -1423,7 +1417,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="B18">
         <v>0.95</v>
@@ -1431,7 +1425,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B19">
         <v>0.95</v>
@@ -1439,7 +1433,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B20">
         <v>0.95</v>
@@ -1447,7 +1441,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="B21">
         <v>0.95</v>
@@ -1455,7 +1449,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B22">
         <v>0.95</v>
@@ -1463,7 +1457,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B23">
         <v>0.95</v>
@@ -1471,7 +1465,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="B24">
         <v>0.95</v>
@@ -1479,7 +1473,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="B25">
         <v>0.95</v>
@@ -1487,7 +1481,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B26">
         <v>0.95</v>
@@ -1495,7 +1489,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="B27">
         <v>0.95</v>
@@ -1503,7 +1497,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="B28">
         <v>0.95</v>
@@ -1511,7 +1505,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="B29">
         <v>0.95</v>
@@ -1519,7 +1513,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B30">
         <v>0.95</v>
@@ -1527,7 +1521,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="B31">
         <v>0.95</v>
@@ -1535,7 +1529,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="B32">
         <v>0.95</v>
@@ -1543,7 +1537,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B33">
         <v>0.95</v>
@@ -1551,7 +1545,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B34">
         <v>0.95</v>
@@ -1559,7 +1553,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="B35">
         <v>0.95</v>
@@ -1567,7 +1561,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B36">
         <v>0.95</v>
@@ -1582,23 +1576,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1609,7 +1601,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1620,7 +1612,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1631,7 +1623,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1642,7 +1634,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1653,7 +1645,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1664,7 +1656,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1675,7 +1667,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1686,7 +1678,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1697,7 +1689,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1708,7 +1700,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1719,7 +1711,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1730,7 +1722,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1741,7 +1733,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1752,7 +1744,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1763,7 +1755,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1774,7 +1766,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1785,7 +1777,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1796,7 +1788,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1807,7 +1799,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1818,7 +1810,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1829,7 +1821,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1840,7 +1832,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1851,7 +1843,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1862,7 +1854,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1873,7 +1865,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1884,7 +1876,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1895,7 +1887,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1906,7 +1898,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1917,7 +1909,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1928,7 +1920,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1939,7 +1931,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1950,7 +1942,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1961,7 +1953,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1972,7 +1964,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="B36">
         <v>1</v>

</xml_diff>